<commit_message>
pmi data is completion
</commit_message>
<xml_diff>
--- a/pmi/comments.xlsx
+++ b/pmi/comments.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,9 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -425,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,10 +445,8 @@
           <t>Industry</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>WHAT RESPONDENTS ARE SAYING</t>
-        </is>
+      <c r="B1" s="2" t="n">
+        <v>45139</v>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
@@ -452,6 +456,36 @@
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>2023-10-01</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2024-01-01</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>2024-02-01</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>2024-03-01</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
         </is>
       </c>
     </row>
@@ -476,6 +510,36 @@
           <t>Markets remain tough, and we have focused more resources on sales and marketing to drive greater sales and new market penetration with our devices. Lots of leadership focus on what we can do in the near term that will also support long-term company goals.</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Economy appears to be slowing dramatically. Customer orders are pushing out, and all efforts are being made to right-size inventory levels, both to mitigate carrying costs on pushed-out orders and to load up on inventory where costs are exploding, like cold-rolled steel.</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Anticipation of the U.S. Federal Reserve holding off on interest-rate changes will encourage more companies to spend on capital investments again. As budgets get approval after the start of the calendar year, this should help drive investment and increase manufacturing activity once again.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>U.S. economic outlook is affecting customer orders, and the current backlog is quite low compared to past quarters. Waiting on potential improvements from the CHIPS and Science Act.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Customer softness continues in China, Japan and Europe.</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Demand remains soft, but optimism is high that orders are 'just on the horizon.' Expectations are for a strong second quarter. Supply chain issues are minimal, with only semiconductors and select electronic parts being an issue.</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Some small indications of market improvement in China for our instruments and technology. Recovery is still slower than we had hoped, and macroeconomic uncertainty remains in Europe and the Middle East, as well as domestically in the U.S. with ongoing inflationary pressures and anticipation for the (upcoming) election.</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -498,6 +562,36 @@
           <t>Economy absolutely slowing down. Less optimism regarding the first quarter of 2024.</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Starting to feel softening in the economy, with labor still a challenge to backfill critical roles. The 2024 forecast looks challenging, specially from a cost perspective.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Overall, order intake has picked up over the last quarter and a backlog of projects is beginning to accumulate.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>The start of 2024 looks good. Sales are above expectations, and costs are mostly stable. A few commodities are up in cost due to supply shortages. Many previously short commodities market positions have corrected themselves. There is a real short-term increase in the cost of international freight.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Currently seeing increasing sales in our business. Most delivery dates are in the second quarter of 2024.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Performance continues to defy projections of a downturn in activity. Demand remains strong, and the pipeline for orders is robust.</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Conditions are improving as demand is starting to recover. Costs continue to be a major concern as suppliers that rapidly increased prices in the follow-up from COVID-19 are slow to return to pre-pandemic levels.</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -520,6 +614,36 @@
           <t>Backlog is starting to dip a bit. We're hearing of cutbacks in 2024 ordering, but it's still very strong compared to historical averages.</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Nearly all microchip supply issues have been resolved, finally bringing an end to the three-year chip shortage. Material prices are remaining relatively flat. Supply chain issues continue in several areas, resulting from difficulties during the United Auto Workers (UAW) strike.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Demand is up across the board. We are starting to see back orders grow again.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>The commercial vehicle market appears to be retracting a bit in 2024 compared to last year. Forecast sales have decreased slightly in most product segments, with only limited growth related to customers' competitive sourcing and moves to new technology. Most supply chains, including for semiconductors, have stabilized, with the only major escalation now being transit through the Red Sea.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>The first quarter will be slower due to some customer order changes, but we are expecting the rest of 2024 to be strong. We may increase our growth projections.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Expecting to see orders and production pick up for the second quarter. Suppliers are working with us to help drive costs down, which will help improve the margin for the rest of the year and deliver growth in 2025.</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Sales continue to exceed expectations in 2024. The forecasted dip in commercial vehicle production volumes appears to be avoided. Operational output is still strong, and the supply chain has the capacity to support. International supply chain risks have been minimized, but the frequency of supplier insolvencies or bankruptcies appears to be increasing.</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -542,6 +666,36 @@
           <t>Markets appear to have slightly slowed. Certain commodities remain high.</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Our executives have requested that we bring down inventory levels considerably, and it has started causing customer shortages. Both finished goods, and low inventories of raw and packing materials are creating issues in fulfilling customer demand, and in some cases causing serious (production) delays.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Commodity costs are decreasing. Supply is readily available, and customers are still ordering to last year's volumes.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Business continues to stabilize. Cash flow will be tight in 2024.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Typical first quarter volume drops from fourth quarter high volumes. Additional distribution has allowed us to maintain consistent production shifts.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Commodity prices continue to hold steady.</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Order flow has stabilized. It took some customers longer to replenish their supply chain network after the fourth-quarter rush we commonly have. Order rates are expected to remain stable through August.</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -560,6 +714,36 @@
           <t>A slow fourth quarter, and we're clearly in a mild industry recession. However, demand is down less than 5 percent, and customer confidence of a recovery in the second half of 2024 is solid. Supplier deliveries are stable, and suppliers are seeking more work. But they're not yet willing to adjust prices to compete for it.</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Automotive sales still impacted by UAW strike. Still waiting for orders to come in, and we also need to work down inventory levels that increased during the strike period. This will most likely happen in December.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>We are forecasting a somewhat strong year for 2024. We're currently mildly optimistic for how next year will play out.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Good start to the year. We had budgeted a 3.5-percent increase over 2023. We expect it to be a challenging year. Currently, orders are positive in our automotive OEM and automotive aftermarket business. Our industrial business sector is looking weak at the moment. Still expect to achieve budget forecasts through the first quarter. (We) feel January is running high for automotive because at the end of December, many OEMs cancelled the last few weeks of orders to reduce inventory levels.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Customer orders are steady, neither up nor down compared to last month. This steady state is what we budgeted and forecast. We are forecasting business to increase 2 percent to 4 percent over the next couple of months.</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Business is still strong — we are meeting and exceeding our forecasts. So far, we're not hearing anything negative with our customers as far as ongoing business is concerned — it's the same for raw material suppliers, nothing negative.</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Business is slowing down — it has been a gradual decline for the last several months. We are not seeing new orders at last year's level, or at this year's budgeted levels.</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -578,6 +762,36 @@
           <t>Seeing a slowdown on bookings, and our backlog is down to five days from 15 weeks earlier this year.</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>The end of the major construction season and an early pullback in customer capital expenditures purchases have resulted in a lower backlog in the fourth quarter.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Business is slowing. Finished goods inventories are growing.</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>December sales were very strong but slower for the first part of January, as was expected. We expect to see steady sales going forward, if the (U.S. Federal Reserve) continues to hold rates and suggests a rate cut in the future.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Demand has finally picked up, with customer orders more closely resembling typical January and February levels. January was up 22 percent compared to December; February up 26 percent compared to January.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Noticing an increase in suppliers' selectiveness regarding orders they quote and take. Additionally, there's been a noticeable increase in manufacturing companies targeted for acquisition by larger entities (established companies, investment firms and the like).</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Market conditions have definitely softened. Thankfully, our backlog is strong and will get us through the year. When conditions improve as expected later this year, we will be in a good position to continue building the business. We are a manufacturer of automated packaging equipment for the food and beverage industry, and with a continued shortage of workers, our customers are requiring more and more automation.</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -592,6 +806,28 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Finishing the year similar to 2022; however, 2023 was more erratic. Working to restore inventory position to ensure we have appropriate safety stock.</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Demand continues to be slow. Reduction from the second half of 2023 has continued into this year. We are adjusting production to match demand.</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>We are experiencing increased sales, which is putting pressure on the plant and assembly to meet new customer demand.</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>There has been a lot of volatility in sales. On average, our sales look flat, but the volatility is concerning.</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -610,6 +846,28 @@
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Customer orders have pushed into the first quarter of 2024, resulting in inflated end-of-year inventory.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Business conditions are good; sales and production are tracking in accordance with forecasts.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Order backlog, which was at historically high levels, is diminishing due to supply chain improvements and slight slowdown of orders.</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Business outlook overall is stable. Working through customer backlog with some raw material lead times improving.</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -624,6 +882,16 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>As an energy-intensive manufacturer, energy pricing continues to be a concern for our business. The move to electrification has increased demand, and supply is not stable because we're not in an ideal geography for wind and solar power.</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -642,6 +910,16 @@
           <t>Orders continue to increase in some sectors. Construction industry-related products/orders are slowing down.</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>The major factor affecting our business is the uncertainty of the Federal Reserve's handling of interest rates, which will affect our customers' businesses, thereby affecting ours.</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -664,6 +942,36 @@
           <t>Despite the ongoing United Auto Workers (UAW) strike, there's a firmness and pickup in orders for the rest of the fourth quarter.</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Customers back online after the UAW strike. Consuming inventory that was built as a strike bank. Still (having) issues with hiring quality candidates for both hourly and salaried positions. Current inventory levels are too high, but the order book remains strong.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>We are seeing stronger demand from our American Automotive OEM customers now that the United Auto Workers (UAW) strike has been resolved. Looking at a very strong first quarter of 2024.</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Current industry conditions are positive; however, a note of caution as we see potential headwinds with downward price movements in the coming months.</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>The month seems to be getting stronger with each passing day and week. Lots of market volatility —pricing flat to downward. It will be interesting to see how the last days of the month play out, as indications seem to be all over the place.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Continue to experience a softness in the industrial sector. There is optimism that order activity will increase in the late second quarter, leading to improvement in this segment for the second half of the year. The aerospace and defense market is continuing to ramp up, and demand is outpacing supply in our supply chain.</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Business is stable, and orders have been consistent. We're quoting new business for the factory, and automotive builds continue at averages but not near maximum outputs. Workforce is stable, with the turnover ratio dropping considerably. Salaries and hourly rates increasing to meet inflationary pressures.</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -678,6 +986,24 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Elevated financing costs have dampened demand for residential investment. Our business has been negatively impacted through reduced new orders for our products and services. We are purchasing less for production and finished goods inventories.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Higher financing costs have diminished demand for residential investment. Customers are delaying a portion of their plans until borrowing costs are reduced. We are impacted with reduced new orders, diminished backlog of orders and uncertain short-term demand for products and services.</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Business activity is up. Many manufacturers are anticipating better business in the second quarter and much better in the third quarter. They are reporting that second-quarter bookings are just starting to ramp up.</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -692,6 +1018,12 @@
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -710,6 +1042,24 @@
           <t>Commercial constructions continue to remain ahead of 2022. We have some concern over 2024 regarding inflation, as well as gas and oil pricing potentially slowing down building.</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>(Our situation is) good but guarded, as next year is hard to predict. There are undertones of uncertainty in the market and the impact of inflation on maintenance and project costs has become apparent.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>We reflected on 2023 for maybe a minute and turned the page forward to 2024. Weather in January caused several operations to be idle, and shipments were affected.</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Business remained strong through the first quarter and has started strong for the second quarter. Commercial construction is still going well but on a regional basis, with the Southeast the strongest.</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -728,6 +1078,16 @@
           <t>Demand for raw materials/chemicals appears to be stable heading into the fourth quarter.</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>The potential aftermaths of the presidential election are beginning to impact conversations and negotiations of long-term agreements/contracts.</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -742,6 +1102,16 @@
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Remarkable slowdown in business in December. January has picked up, but not to previous-year levels.</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -756,6 +1126,12 @@
           <t>Business is decent — not great, but steady and solid. We are meeting our sales and margin goals, but it's definitely hard to guess the future.</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>